<commit_message>
adding temperature data to excel export
</commit_message>
<xml_diff>
--- a/analysis results.xlsx
+++ b/analysis results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:M15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -474,6 +474,26 @@
           <t>sum rainfall in critical quarter 2017-2021</t>
         </is>
       </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Mean_T_anom_2002-2007</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Mean_T_anom_2007-2012</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Mean_T_anom_2012-2017</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Mean_T_anom_2017-2022</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -505,6 +525,18 @@
       <c r="I2" t="n">
         <v>147.6066691080729</v>
       </c>
+      <c r="J2" t="n">
+        <v>1.027534365653992</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0.5953571796417236</v>
+      </c>
+      <c r="L2" t="n">
+        <v>0.9207971096038818</v>
+      </c>
+      <c r="M2" t="n">
+        <v>1.407952666282654</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -536,6 +568,18 @@
       <c r="I3" t="n">
         <v>227.7799886067708</v>
       </c>
+      <c r="J3" t="n">
+        <v>0.1529367417097092</v>
+      </c>
+      <c r="K3" t="n">
+        <v>-0.2098842114210129</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0.1759693473577499</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0.476120263338089</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -567,6 +611,18 @@
       <c r="I4" t="n">
         <v>202.8800048828125</v>
       </c>
+      <c r="J4" t="n">
+        <v>0.3213476538658142</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0.2530762851238251</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0.4622536599636078</v>
+      </c>
+      <c r="M4" t="n">
+        <v>0.8613607883453369</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -598,6 +654,18 @@
       <c r="I5" t="n">
         <v>197.5533447265625</v>
       </c>
+      <c r="J5" t="n">
+        <v>0.6876922845840454</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0.4942399561405182</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0.7095251679420471</v>
+      </c>
+      <c r="M5" t="n">
+        <v>1.114517331123352</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -629,6 +697,18 @@
       <c r="I6" t="n">
         <v>165.5533345540365</v>
       </c>
+      <c r="J6" t="n">
+        <v>0.9773463010787964</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0.6907257437705994</v>
+      </c>
+      <c r="L6" t="n">
+        <v>1.033843874931335</v>
+      </c>
+      <c r="M6" t="n">
+        <v>1.462576985359192</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -660,6 +740,18 @@
       <c r="I7" t="n">
         <v>76.57333374023438</v>
       </c>
+      <c r="J7" t="n">
+        <v>0.8976433277130127</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0.5702357888221741</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0.7934548258781433</v>
+      </c>
+      <c r="M7" t="n">
+        <v>1.276681780815125</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
@@ -691,6 +783,18 @@
       <c r="I8" t="n">
         <v>54.8066660563151</v>
       </c>
+      <c r="J8" t="n">
+        <v>0.9124077558517456</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0.5719060897827148</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0.8839142322540283</v>
+      </c>
+      <c r="M8" t="n">
+        <v>1.381705760955811</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
@@ -722,6 +826,18 @@
       <c r="I9" t="n">
         <v>57.56667073567709</v>
       </c>
+      <c r="J9" t="n">
+        <v>0.8915310502052307</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0.4934071600437164</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0.9293677806854248</v>
+      </c>
+      <c r="M9" t="n">
+        <v>1.325136542320251</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
@@ -753,6 +869,18 @@
       <c r="I10" t="n">
         <v>107.6466674804688</v>
       </c>
+      <c r="J10" t="n">
+        <v>0.1984381079673767</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0.1777880936861038</v>
+      </c>
+      <c r="L10" t="n">
+        <v>0.4904373586177826</v>
+      </c>
+      <c r="M10" t="n">
+        <v>0.5138602256774902</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
@@ -784,6 +912,18 @@
       <c r="I11" t="n">
         <v>180.0666707356771</v>
       </c>
+      <c r="J11" t="n">
+        <v>0.2728450894355774</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0.05762287601828575</v>
+      </c>
+      <c r="L11" t="n">
+        <v>0.405795693397522</v>
+      </c>
+      <c r="M11" t="n">
+        <v>0.7220320701599121</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
@@ -815,6 +955,18 @@
       <c r="I12" t="n">
         <v>173.2200113932292</v>
       </c>
+      <c r="J12" t="n">
+        <v>0.3603193163871765</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0.4083164036273956</v>
+      </c>
+      <c r="L12" t="n">
+        <v>0.5908300876617432</v>
+      </c>
+      <c r="M12" t="n">
+        <v>0.8542513251304626</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
@@ -846,6 +998,18 @@
       <c r="I13" t="n">
         <v>55.84666951497396</v>
       </c>
+      <c r="J13" t="n">
+        <v>0.7681716680526733</v>
+      </c>
+      <c r="K13" t="n">
+        <v>0.5500335097312927</v>
+      </c>
+      <c r="L13" t="n">
+        <v>0.9291219711303711</v>
+      </c>
+      <c r="M13" t="n">
+        <v>1.46335780620575</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
@@ -877,6 +1041,18 @@
       <c r="I14" t="n">
         <v>99.8800048828125</v>
       </c>
+      <c r="J14" t="n">
+        <v>0.6368283033370972</v>
+      </c>
+      <c r="K14" t="n">
+        <v>0.9244036078453064</v>
+      </c>
+      <c r="L14" t="n">
+        <v>1.339719653129578</v>
+      </c>
+      <c r="M14" t="n">
+        <v>1.588810563087463</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
@@ -907,6 +1083,18 @@
       </c>
       <c r="I15" t="n">
         <v>62.02666727701823</v>
+      </c>
+      <c r="J15" t="n">
+        <v>0.7681716680526733</v>
+      </c>
+      <c r="K15" t="n">
+        <v>0.5500335097312927</v>
+      </c>
+      <c r="L15" t="n">
+        <v>0.9291219711303711</v>
+      </c>
+      <c r="M15" t="n">
+        <v>1.46335780620575</v>
       </c>
     </row>
   </sheetData>

</xml_diff>